<commit_message>
PAPA Moorings Ingest and Cal sheet update D3
PAPA moorings Deployment 3

Reviewed and made changes to reference designators in cal sheets,
created ingest CSVs.
</commit_message>
<xml_diff>
--- a/GP02HYPM/Omaha_Cal_Info_GP02HYPM_00003.xlsx
+++ b/GP02HYPM/Omaha_Cal_Info_GP02HYPM_00003.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\Ingest sheets\ingestion-csvs\GP02HYPM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="7380" windowWidth="29700" windowHeight="14420"/>
+    <workbookView xWindow="8100" yWindow="7380" windowWidth="29700" windowHeight="14415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -17,12 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -287,49 +287,6 @@
   </si>
   <si>
     <r>
-      <t>GP02HYPM-RI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>M</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>01-00-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SIO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EN000</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>GP02HYPM-WFP02-00-</t>
     </r>
     <r>
@@ -382,17 +339,20 @@
   <si>
     <t>13104-03</t>
   </si>
+  <si>
+    <t>GP02HYPM-GPM01-00-SIOENG000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -714,7 +674,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="199">
+  <cellStyleXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -777,14 +737,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -914,6 +874,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -971,10 +932,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -992,10 +953,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1034,10 +995,10 @@
     <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
@@ -1067,7 +1028,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="57" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1098,7 +1059,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="199">
+  <cellStyles count="200">
     <cellStyle name="Comma 2" xfId="62"/>
     <cellStyle name="Comma 2 2" xfId="63"/>
     <cellStyle name="Comma 2 2 2" xfId="64"/>
@@ -1195,6 +1156,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="15"/>
     <cellStyle name="Normal 11" xfId="16"/>
+    <cellStyle name="Normal 11 2" xfId="199"/>
     <cellStyle name="Normal 12" xfId="17"/>
     <cellStyle name="Normal 13" xfId="18"/>
     <cellStyle name="Normal 14" xfId="57"/>
@@ -1305,12 +1267,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1369,7 +1334,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1404,7 +1369,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1615,29 +1580,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="27" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" style="11" customWidth="1"/>
-    <col min="12" max="12" width="17.1640625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="17.83203125" style="11" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="27" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="11" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" style="11" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" style="11" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="15" customFormat="1" ht="28">
+    <row r="1" spans="1:13" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1672,7 +1637,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="28" customFormat="1">
+    <row r="2" spans="1:13" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>40</v>
       </c>
@@ -1705,48 +1670,48 @@
       <c r="L2" s="38"/>
       <c r="M2" s="38"/>
     </row>
-    <row r="3" spans="1:13" s="28" customFormat="1">
+    <row r="3" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="39"/>
       <c r="E3" s="40"/>
       <c r="F3" s="39"/>
     </row>
-    <row r="4" spans="1:13" customFormat="1"/>
-    <row r="5" spans="1:13" customFormat="1"/>
-    <row r="6" spans="1:13" customFormat="1"/>
-    <row r="7" spans="1:13" customFormat="1"/>
-    <row r="8" spans="1:13" customFormat="1"/>
-    <row r="9" spans="1:13" customFormat="1"/>
-    <row r="10" spans="1:13" s="28" customFormat="1">
+    <row r="4" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:13" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D10" s="39"/>
       <c r="E10" s="40"/>
       <c r="F10" s="39"/>
     </row>
-    <row r="11" spans="1:13" s="28" customFormat="1">
+    <row r="11" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D11" s="39"/>
       <c r="E11" s="40"/>
       <c r="F11" s="39"/>
     </row>
-    <row r="12" spans="1:13" s="28" customFormat="1">
+    <row r="12" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="39"/>
       <c r="E12" s="40"/>
       <c r="F12" s="39"/>
     </row>
-    <row r="13" spans="1:13" s="28" customFormat="1">
+    <row r="13" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="39"/>
       <c r="E13" s="40"/>
       <c r="F13" s="39"/>
     </row>
-    <row r="14" spans="1:13" s="28" customFormat="1">
+    <row r="14" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="39"/>
       <c r="E14" s="40"/>
       <c r="F14" s="39"/>
     </row>
-    <row r="15" spans="1:13" s="28" customFormat="1">
+    <row r="15" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="39"/>
       <c r="E15" s="40"/>
       <c r="F15" s="39"/>
     </row>
-    <row r="16" spans="1:13" s="28" customFormat="1">
+    <row r="16" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="39"/>
       <c r="E16" s="40"/>
       <c r="F16" s="39"/>
@@ -1764,30 +1729,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="18" customWidth="1"/>
-    <col min="8" max="11" width="10.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="18" customWidth="1"/>
+    <col min="8" max="11" width="10.7109375" style="3" customWidth="1"/>
     <col min="12" max="12" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="3"/>
+    <col min="13" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="24" customFormat="1">
+    <row r="1" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1810,7 +1775,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="24" customFormat="1">
+    <row r="2" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="36"/>
       <c r="C2" s="37"/>
@@ -1819,7 +1784,7 @@
       <c r="F2" s="23"/>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1842,7 +1807,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1863,7 +1828,7 @@
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1884,7 +1849,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1905,7 +1870,7 @@
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1928,7 +1893,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1951,7 +1916,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1974,7 +1939,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1997,7 +1962,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="43"/>
       <c r="C11" s="5"/>
@@ -2006,7 +1971,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -2029,7 +1994,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -2049,7 +2014,7 @@
         <v>-144.803</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="43"/>
       <c r="C14" s="5"/>
@@ -2057,7 +2022,7 @@
       <c r="E14" s="17"/>
       <c r="F14" s="18"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -2077,7 +2042,7 @@
         <v>50.079833333333333</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -2097,7 +2062,7 @@
         <v>-144.803</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="43"/>
       <c r="C17" s="5"/>
@@ -2105,7 +2070,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -2125,7 +2090,7 @@
         <v>50.079833333333333</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -2145,7 +2110,7 @@
         <v>-144.803</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="43"/>
       <c r="C20" s="5"/>
@@ -2153,9 +2118,9 @@
       <c r="E20" s="17"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>41</v>
@@ -2164,14 +2129,14 @@
         <v>3</v>
       </c>
       <c r="D21" s="57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G21" s="52"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -2194,7 +2159,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
@@ -2215,7 +2180,7 @@
       </c>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -2236,7 +2201,7 @@
       </c>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -2257,7 +2222,7 @@
       </c>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>9</v>
       </c>
@@ -2280,7 +2245,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
@@ -2303,7 +2268,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
@@ -2325,8 +2290,9 @@
       <c r="G29" s="16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>9</v>
       </c>
@@ -2348,8 +2314,9 @@
       <c r="G30" s="16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="43"/>
       <c r="C31" s="5"/>
@@ -2357,8 +2324,9 @@
       <c r="E31" s="4"/>
       <c r="F31" s="10"/>
       <c r="G31" s="16"/>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" s="52"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -2377,8 +2345,9 @@
       <c r="F32" s="53">
         <v>50.079833333333333</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="52"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
@@ -2397,8 +2366,9 @@
       <c r="F33" s="53">
         <v>-144.803</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="43"/>
       <c r="C34" s="5"/>
@@ -2406,7 +2376,7 @@
       <c r="E34" s="17"/>
       <c r="F34" s="18"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
@@ -2425,8 +2395,9 @@
       <c r="F35" s="53">
         <v>50.079833333333333</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>11</v>
       </c>
@@ -2445,8 +2416,9 @@
       <c r="F36" s="53">
         <v>-144.803</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" s="18"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="43"/>
       <c r="C37" s="5"/>
@@ -2454,7 +2426,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="18"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>12</v>
       </c>
@@ -2474,7 +2446,7 @@
         <v>50.079833333333333</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>12</v>
       </c>
@@ -2494,7 +2466,7 @@
         <v>-144.803</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="48"/>
       <c r="B40" s="43"/>
       <c r="C40" s="5"/>
@@ -2502,9 +2474,9 @@
       <c r="E40" s="17"/>
       <c r="F40" s="18"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>41</v>
@@ -2513,53 +2485,53 @@
         <v>3</v>
       </c>
       <c r="D41" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G41" s="52"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="56" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G43" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="18">
-        <v>3</v>
-      </c>
-      <c r="D43" s="46"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="47" t="s">
+      <c r="H43" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="I43" s="18">
+        <v>3</v>
+      </c>
+      <c r="J43" s="46"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="56" t="s">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G44" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="18">
-        <v>3</v>
-      </c>
-      <c r="D44" s="46"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="47" t="s">
+      <c r="H44" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="I44" s="18">
+        <v>3</v>
+      </c>
+      <c r="J44" s="46"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="45"/>
       <c r="B45" s="42"/>
       <c r="D45" s="46"/>
       <c r="F45" s="18"/>
       <c r="G45" s="47"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>48</v>
       </c>
@@ -2581,7 +2553,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>49</v>
       </c>
@@ -2601,7 +2573,7 @@
         <v>50.079833333333333</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>49</v>
       </c>
@@ -2621,7 +2593,7 @@
         <v>-144.803</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="48"/>
       <c r="B49" s="43"/>
       <c r="C49" s="5"/>
@@ -2629,9 +2601,9 @@
       <c r="E49" s="7"/>
       <c r="F49" s="18"/>
     </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="49" t="s">
-        <v>50</v>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>41</v>
@@ -2644,23 +2616,16 @@
       </c>
       <c r="E50" s="51"/>
       <c r="F50" s="51"/>
-      <c r="G50" s="52"/>
-    </row>
-    <row r="51" spans="1:7">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="49"/>
       <c r="C51" s="3"/>
       <c r="D51" s="50"/>
       <c r="E51" s="51"/>
       <c r="F51" s="51"/>
-      <c r="G51" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>